<commit_message>
mise en place des traces
mise en oeuvre des traces
modification des traces
modificatiuon des ensembles
</commit_message>
<xml_diff>
--- a/RuleCout2.xlsx
+++ b/RuleCout2.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="66">
   <si>
     <t>pas cher du tout éco</t>
   </si>
@@ -51,9 +51,6 @@
     <t xml:space="preserve">bon marché </t>
   </si>
   <si>
-    <t xml:space="preserve">peu onéreux </t>
-  </si>
-  <si>
     <t xml:space="preserve">moins de vingt euros </t>
   </si>
   <si>
@@ -63,9 +60,6 @@
     <t xml:space="preserve">avantageux </t>
   </si>
   <si>
-    <t xml:space="preserve">je ne suis pas très riche </t>
-  </si>
-  <si>
     <t>éco</t>
   </si>
   <si>
@@ -114,9 +108,6 @@
     <t xml:space="preserve">je m’en fiche </t>
   </si>
   <si>
-    <t xml:space="preserve">c’est pas un problème </t>
-  </si>
-  <si>
     <t xml:space="preserve">gastronomique </t>
   </si>
   <si>
@@ -162,9 +153,6 @@
     <t>moyen de gamme</t>
   </si>
   <si>
-    <t>y'a pas de pb</t>
-  </si>
-  <si>
     <t>aucun problème d'argent</t>
   </si>
   <si>
@@ -184,6 +172,51 @@
   </si>
   <si>
     <t xml:space="preserve">menu pas cher le midi </t>
+  </si>
+  <si>
+    <t>pas cher</t>
+  </si>
+  <si>
+    <t>très haut de gamme</t>
+  </si>
+  <si>
+    <t>vraiment luxueux</t>
+  </si>
+  <si>
+    <t>très bas de gamme</t>
+  </si>
+  <si>
+    <t>pas trop cher</t>
+  </si>
+  <si>
+    <t>très économique</t>
+  </si>
+  <si>
+    <t>peu onéreux</t>
+  </si>
+  <si>
+    <t>bon</t>
+  </si>
+  <si>
+    <t>le meilleur des meilleurs</t>
+  </si>
+  <si>
+    <t>vraiment bon</t>
+  </si>
+  <si>
+    <t>plutôt bien</t>
+  </si>
+  <si>
+    <t>plutôt pas mal</t>
+  </si>
+  <si>
+    <t>un restau de qualité</t>
+  </si>
+  <si>
+    <t>qualité</t>
+  </si>
+  <si>
+    <t>plutôt pas cher</t>
   </si>
 </sst>
 </file>
@@ -1024,7 +1057,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B52"/>
+  <dimension ref="A1:B65"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -1035,421 +1068,528 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>40</v>
+        <v>46</v>
       </c>
       <c r="B1" t="s">
-        <v>41</v>
+        <v>13</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>0</v>
+        <v>44</v>
       </c>
       <c r="B2" t="s">
-        <v>15</v>
+        <v>36</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="B3" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>3</v>
+        <v>47</v>
       </c>
       <c r="B5" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>4</v>
+        <v>58</v>
       </c>
       <c r="B6" t="s">
-        <v>15</v>
+        <v>36</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>50</v>
+        <v>9</v>
       </c>
       <c r="B7" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>43</v>
+        <v>16</v>
       </c>
       <c r="B8" t="s">
-        <v>15</v>
+        <v>45</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>5</v>
+        <v>41</v>
       </c>
       <c r="B9" t="s">
-        <v>15</v>
+        <v>36</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>51</v>
+        <v>13</v>
       </c>
       <c r="B10" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>6</v>
+        <v>39</v>
       </c>
       <c r="B11" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>7</v>
+        <v>29</v>
       </c>
       <c r="B12" t="s">
-        <v>15</v>
+        <v>36</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>15</v>
+        <v>30</v>
       </c>
       <c r="B13" t="s">
-        <v>15</v>
+        <v>36</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>42</v>
+        <v>33</v>
       </c>
       <c r="B14" t="s">
-        <v>15</v>
+        <v>36</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>8</v>
+        <v>28</v>
       </c>
       <c r="B15" t="s">
-        <v>15</v>
+        <v>36</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>9</v>
+        <v>27</v>
       </c>
       <c r="B16" t="s">
-        <v>15</v>
+        <v>36</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>10</v>
+        <v>19</v>
       </c>
       <c r="B17" t="s">
-        <v>15</v>
+        <v>36</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>11</v>
+        <v>59</v>
       </c>
       <c r="B18" t="s">
-        <v>15</v>
+        <v>36</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>53</v>
+        <v>24</v>
       </c>
       <c r="B19" t="s">
-        <v>15</v>
+        <v>36</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>54</v>
+        <v>25</v>
       </c>
       <c r="B20" t="s">
-        <v>15</v>
+        <v>36</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>12</v>
+        <v>20</v>
       </c>
       <c r="B21" t="s">
-        <v>15</v>
+        <v>36</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>13</v>
+        <v>50</v>
       </c>
       <c r="B22" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>14</v>
+        <v>5</v>
       </c>
       <c r="B23" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="B24" t="s">
-        <v>49</v>
+        <v>36</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>16</v>
+        <v>4</v>
       </c>
       <c r="B25" t="s">
-        <v>49</v>
+        <v>13</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="B26" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>18</v>
+        <v>49</v>
       </c>
       <c r="B27" t="s">
-        <v>49</v>
+        <v>13</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="B28" t="s">
-        <v>49</v>
+        <v>13</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>20</v>
+        <v>43</v>
       </c>
       <c r="B29" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>47</v>
+        <v>18</v>
       </c>
       <c r="B30" t="s">
-        <v>39</v>
+        <v>45</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="B31" t="s">
-        <v>39</v>
+        <v>13</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>45</v>
+        <v>8</v>
       </c>
       <c r="B32" t="s">
-        <v>39</v>
+        <v>13</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>21</v>
+        <v>0</v>
       </c>
       <c r="B33" t="s">
-        <v>39</v>
+        <v>13</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>22</v>
+        <v>55</v>
       </c>
       <c r="B34" t="s">
-        <v>39</v>
+        <v>13</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>23</v>
+        <v>15</v>
       </c>
       <c r="B35" t="s">
-        <v>39</v>
+        <v>45</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
       <c r="B36" t="s">
-        <v>39</v>
+        <v>45</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>25</v>
+        <v>57</v>
       </c>
       <c r="B37" t="s">
-        <v>39</v>
+        <v>13</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>26</v>
+        <v>31</v>
       </c>
       <c r="B38" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>27</v>
+        <v>61</v>
       </c>
       <c r="B39" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>28</v>
+        <v>42</v>
       </c>
       <c r="B40" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>29</v>
+        <v>42</v>
       </c>
       <c r="B41" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>30</v>
+        <v>65</v>
       </c>
       <c r="B42" t="s">
-        <v>39</v>
+        <v>13</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>31</v>
+        <v>62</v>
       </c>
       <c r="B43" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>44</v>
+        <v>6</v>
       </c>
       <c r="B44" t="s">
-        <v>39</v>
+        <v>13</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>52</v>
+        <v>64</v>
       </c>
       <c r="B45" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>32</v>
+        <v>21</v>
       </c>
       <c r="B46" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>33</v>
+        <v>22</v>
       </c>
       <c r="B47" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="B48" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>35</v>
+        <v>54</v>
       </c>
       <c r="B49" t="s">
-        <v>39</v>
+        <v>13</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>36</v>
+        <v>1</v>
       </c>
       <c r="B50" t="s">
-        <v>39</v>
+        <v>13</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>37</v>
+        <v>56</v>
       </c>
       <c r="B51" t="s">
-        <v>39</v>
+        <v>13</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>38</v>
+        <v>52</v>
       </c>
       <c r="B52" t="s">
-        <v>39</v>
+        <v>36</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>52</v>
+      </c>
+      <c r="B53" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>2</v>
+      </c>
+      <c r="B54" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>34</v>
+      </c>
+      <c r="B55" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
+        <v>7</v>
+      </c>
+      <c r="B56" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
+        <v>32</v>
+      </c>
+      <c r="B57" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
+        <v>63</v>
+      </c>
+      <c r="B58" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
+        <v>26</v>
+      </c>
+      <c r="B59" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A60" t="s">
+        <v>11</v>
+      </c>
+      <c r="B60" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A61" t="s">
+        <v>35</v>
+      </c>
+      <c r="B61" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A62" t="s">
+        <v>23</v>
+      </c>
+      <c r="B62" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A63" t="s">
+        <v>60</v>
+      </c>
+      <c r="B63" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A64" t="s">
+        <v>53</v>
+      </c>
+      <c r="B64" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A65" t="s">
+        <v>40</v>
+      </c>
+      <c r="B65" t="s">
+        <v>13</v>
       </c>
     </row>
   </sheetData>
+  <sortState ref="A1:B65">
+    <sortCondition ref="A1:A65"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
entre 5 et 15
record à 78,10 %
ajouter exemple entre 5 et 15
</commit_message>
<xml_diff>
--- a/RuleCout2.xlsx
+++ b/RuleCout2.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="69">
   <si>
     <t>pas cher du tout éco</t>
   </si>
@@ -217,6 +217,15 @@
   </si>
   <si>
     <t>plutôt pas cher</t>
+  </si>
+  <si>
+    <t>entre 10 et 20</t>
+  </si>
+  <si>
+    <t>moins de quinze</t>
+  </si>
+  <si>
+    <t>jusqu'à cinquante</t>
   </si>
 </sst>
 </file>
@@ -1057,9 +1066,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B65"/>
+  <dimension ref="A1:B69"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:XFD1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1068,10 +1079,10 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>46</v>
+        <v>37</v>
       </c>
       <c r="B1" t="s">
-        <v>13</v>
+        <v>38</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
@@ -1084,31 +1095,31 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>12</v>
+        <v>58</v>
       </c>
       <c r="B3" t="s">
-        <v>13</v>
+        <v>36</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>3</v>
+        <v>41</v>
       </c>
       <c r="B4" t="s">
-        <v>13</v>
+        <v>36</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>47</v>
+        <v>29</v>
       </c>
       <c r="B5" t="s">
-        <v>13</v>
+        <v>36</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>58</v>
+        <v>30</v>
       </c>
       <c r="B6" t="s">
         <v>36</v>
@@ -1116,23 +1127,23 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>9</v>
+        <v>33</v>
       </c>
       <c r="B7" t="s">
-        <v>13</v>
+        <v>36</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>16</v>
+        <v>28</v>
       </c>
       <c r="B8" t="s">
-        <v>45</v>
+        <v>36</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>41</v>
+        <v>27</v>
       </c>
       <c r="B9" t="s">
         <v>36</v>
@@ -1140,23 +1151,23 @@
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="B10" t="s">
-        <v>13</v>
+        <v>36</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>39</v>
+        <v>59</v>
       </c>
       <c r="B11" t="s">
-        <v>13</v>
+        <v>36</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="B12" t="s">
         <v>36</v>
@@ -1164,7 +1175,7 @@
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="B13" t="s">
         <v>36</v>
@@ -1172,7 +1183,7 @@
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>33</v>
+        <v>20</v>
       </c>
       <c r="B14" t="s">
         <v>36</v>
@@ -1180,7 +1191,7 @@
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>28</v>
+        <v>48</v>
       </c>
       <c r="B15" t="s">
         <v>36</v>
@@ -1188,7 +1199,7 @@
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="B16" t="s">
         <v>36</v>
@@ -1196,7 +1207,7 @@
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>19</v>
+        <v>61</v>
       </c>
       <c r="B17" t="s">
         <v>36</v>
@@ -1204,7 +1215,7 @@
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>59</v>
+        <v>42</v>
       </c>
       <c r="B18" t="s">
         <v>36</v>
@@ -1212,7 +1223,7 @@
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>24</v>
+        <v>42</v>
       </c>
       <c r="B19" t="s">
         <v>36</v>
@@ -1220,7 +1231,7 @@
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>25</v>
+        <v>62</v>
       </c>
       <c r="B20" t="s">
         <v>36</v>
@@ -1228,7 +1239,7 @@
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>20</v>
+        <v>64</v>
       </c>
       <c r="B21" t="s">
         <v>36</v>
@@ -1236,23 +1247,23 @@
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>50</v>
+        <v>21</v>
       </c>
       <c r="B22" t="s">
-        <v>13</v>
+        <v>36</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>5</v>
+        <v>22</v>
       </c>
       <c r="B23" t="s">
-        <v>13</v>
+        <v>36</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="B24" t="s">
         <v>36</v>
@@ -1260,79 +1271,79 @@
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>4</v>
+        <v>52</v>
       </c>
       <c r="B25" t="s">
-        <v>13</v>
+        <v>36</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>14</v>
+        <v>34</v>
       </c>
       <c r="B26" t="s">
-        <v>45</v>
+        <v>36</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>49</v>
+        <v>32</v>
       </c>
       <c r="B27" t="s">
-        <v>13</v>
+        <v>36</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>10</v>
+        <v>63</v>
       </c>
       <c r="B28" t="s">
-        <v>13</v>
+        <v>36</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>43</v>
+        <v>26</v>
       </c>
       <c r="B29" t="s">
-        <v>45</v>
+        <v>36</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>18</v>
+        <v>35</v>
       </c>
       <c r="B30" t="s">
-        <v>45</v>
+        <v>36</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>51</v>
+        <v>23</v>
       </c>
       <c r="B31" t="s">
-        <v>13</v>
+        <v>36</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>8</v>
+        <v>60</v>
       </c>
       <c r="B32" t="s">
-        <v>13</v>
+        <v>36</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>0</v>
+        <v>53</v>
       </c>
       <c r="B33" t="s">
-        <v>13</v>
+        <v>36</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>55</v>
+        <v>46</v>
       </c>
       <c r="B34" t="s">
         <v>13</v>
@@ -1340,23 +1351,23 @@
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="B35" t="s">
-        <v>45</v>
+        <v>13</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>17</v>
+        <v>3</v>
       </c>
       <c r="B36" t="s">
-        <v>45</v>
+        <v>13</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>57</v>
+        <v>47</v>
       </c>
       <c r="B37" t="s">
         <v>13</v>
@@ -1364,39 +1375,39 @@
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>31</v>
+        <v>9</v>
       </c>
       <c r="B38" t="s">
-        <v>36</v>
+        <v>13</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>61</v>
+        <v>13</v>
       </c>
       <c r="B39" t="s">
-        <v>36</v>
+        <v>13</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="B40" t="s">
-        <v>36</v>
+        <v>13</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>42</v>
+        <v>50</v>
       </c>
       <c r="B41" t="s">
-        <v>36</v>
+        <v>13</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>65</v>
+        <v>5</v>
       </c>
       <c r="B42" t="s">
         <v>13</v>
@@ -1404,15 +1415,15 @@
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>62</v>
+        <v>4</v>
       </c>
       <c r="B43" t="s">
-        <v>36</v>
+        <v>13</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>6</v>
+        <v>49</v>
       </c>
       <c r="B44" t="s">
         <v>13</v>
@@ -1420,39 +1431,39 @@
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>64</v>
+        <v>10</v>
       </c>
       <c r="B45" t="s">
-        <v>36</v>
+        <v>13</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>21</v>
+        <v>51</v>
       </c>
       <c r="B46" t="s">
-        <v>36</v>
+        <v>13</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>22</v>
+        <v>8</v>
       </c>
       <c r="B47" t="s">
-        <v>36</v>
+        <v>13</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>37</v>
+        <v>0</v>
       </c>
       <c r="B48" t="s">
-        <v>38</v>
+        <v>13</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="B49" t="s">
         <v>13</v>
@@ -1460,7 +1471,7 @@
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>1</v>
+        <v>57</v>
       </c>
       <c r="B50" t="s">
         <v>13</v>
@@ -1468,7 +1479,7 @@
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>56</v>
+        <v>65</v>
       </c>
       <c r="B51" t="s">
         <v>13</v>
@@ -1476,23 +1487,23 @@
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>52</v>
+        <v>6</v>
       </c>
       <c r="B52" t="s">
-        <v>36</v>
+        <v>13</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="B53" t="s">
-        <v>36</v>
+        <v>13</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B54" t="s">
         <v>13</v>
@@ -1500,15 +1511,15 @@
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>34</v>
+        <v>56</v>
       </c>
       <c r="B55" t="s">
-        <v>36</v>
+        <v>13</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="B56" t="s">
         <v>13</v>
@@ -1516,79 +1527,111 @@
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>32</v>
+        <v>7</v>
       </c>
       <c r="B57" t="s">
-        <v>36</v>
+        <v>13</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>63</v>
+        <v>11</v>
       </c>
       <c r="B58" t="s">
-        <v>36</v>
+        <v>13</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>26</v>
+        <v>40</v>
       </c>
       <c r="B59" t="s">
-        <v>36</v>
+        <v>13</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="B60" t="s">
-        <v>13</v>
+        <v>45</v>
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>35</v>
+        <v>14</v>
       </c>
       <c r="B61" t="s">
-        <v>36</v>
+        <v>45</v>
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>23</v>
+        <v>43</v>
       </c>
       <c r="B62" t="s">
-        <v>36</v>
+        <v>45</v>
       </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>60</v>
+        <v>18</v>
       </c>
       <c r="B63" t="s">
-        <v>36</v>
+        <v>45</v>
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>53</v>
+        <v>15</v>
       </c>
       <c r="B64" t="s">
-        <v>36</v>
+        <v>45</v>
       </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>40</v>
+        <v>17</v>
       </c>
       <c r="B65" t="s">
-        <v>13</v>
+        <v>45</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A66" t="s">
+        <v>66</v>
+      </c>
+      <c r="B66" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A67" t="s">
+        <v>67</v>
+      </c>
+      <c r="B67" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A68" t="s">
+        <v>68</v>
+      </c>
+      <c r="B68" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A69" t="s">
+        <v>14</v>
+      </c>
+      <c r="B69" t="s">
+        <v>45</v>
       </c>
     </row>
   </sheetData>
-  <sortState ref="A1:B65">
-    <sortCondition ref="A1:A65"/>
+  <sortState ref="A2:B65">
+    <sortCondition ref="B2:B65"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>